<commit_message>
Ran Sine2 values and updated log
</commit_message>
<xml_diff>
--- a/Simulink/logs/DryLUPAlog.xlsx
+++ b/Simulink/logs/DryLUPAlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\LUPA\Simulink\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860E2A34-CDEC-49F2-9615-8DEE340D383A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA2C2D7-F0E2-4BB1-8385-B023A5845BE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28704" yWindow="-96" windowWidth="28992" windowHeight="15792" xr2:uid="{C0973FDA-A24E-4A37-9D57-25AD59878F79}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="55">
   <si>
     <t>DryLUPA log</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Chirp2</t>
+  </si>
+  <si>
+    <t>Updated to MATLAB/Simulink R2022a</t>
   </si>
 </sst>
 </file>
@@ -548,8 +551,8 @@
   <dimension ref="A1:H445"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B153" sqref="B153"/>
+      <pane ySplit="2" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B161" sqref="B161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3329,7 +3332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>44628</v>
       </c>
@@ -3346,7 +3349,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>44637</v>
       </c>
@@ -3363,7 +3366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>44637</v>
       </c>
@@ -3380,7 +3383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>44638</v>
       </c>
@@ -3397,7 +3400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>44638</v>
       </c>
@@ -3414,7 +3417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>44638</v>
       </c>
@@ -3431,35 +3434,153 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" s="1"/>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A152" s="1"/>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" s="1"/>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A154" s="1"/>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A155" s="1"/>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A156" s="1"/>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A157" s="1"/>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A158" s="1"/>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A159" s="1"/>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A160" s="1"/>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154" s="1">
+        <v>44641</v>
+      </c>
+      <c r="B154" t="s">
+        <v>50</v>
+      </c>
+      <c r="C154">
+        <v>6</v>
+      </c>
+      <c r="D154">
+        <v>4</v>
+      </c>
+      <c r="E154">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155" s="1">
+        <v>44641</v>
+      </c>
+      <c r="B155" t="s">
+        <v>51</v>
+      </c>
+      <c r="C155">
+        <v>2</v>
+      </c>
+      <c r="D155">
+        <v>0.5</v>
+      </c>
+      <c r="E155">
+        <v>1</v>
+      </c>
+      <c r="F155">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156" s="1">
+        <v>44641</v>
+      </c>
+      <c r="B156" t="s">
+        <v>51</v>
+      </c>
+      <c r="C156">
+        <v>3</v>
+      </c>
+      <c r="D156">
+        <v>0.5</v>
+      </c>
+      <c r="E156">
+        <v>1</v>
+      </c>
+      <c r="F156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A157" s="1">
+        <v>44641</v>
+      </c>
+      <c r="B157" t="s">
+        <v>51</v>
+      </c>
+      <c r="C157">
+        <v>4</v>
+      </c>
+      <c r="D157">
+        <v>0.5</v>
+      </c>
+      <c r="E157">
+        <v>1</v>
+      </c>
+      <c r="F157">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A158" s="1">
+        <v>44641</v>
+      </c>
+      <c r="B158" t="s">
+        <v>51</v>
+      </c>
+      <c r="C158">
+        <v>5</v>
+      </c>
+      <c r="D158">
+        <v>0.5</v>
+      </c>
+      <c r="E158">
+        <v>1</v>
+      </c>
+      <c r="F158">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159" s="1">
+        <v>44641</v>
+      </c>
+      <c r="B159" t="s">
+        <v>51</v>
+      </c>
+      <c r="C159">
+        <v>6</v>
+      </c>
+      <c r="D159">
+        <v>0.5</v>
+      </c>
+      <c r="E159">
+        <v>1</v>
+      </c>
+      <c r="F159">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160" s="1">
+        <v>44641</v>
+      </c>
+      <c r="B160" t="s">
+        <v>51</v>
+      </c>
+      <c r="C160">
+        <v>7</v>
+      </c>
+      <c r="D160">
+        <v>1.5</v>
+      </c>
+      <c r="E160">
+        <v>3</v>
+      </c>
+      <c r="F160">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" s="1"/>

</xml_diff>

<commit_message>
added commanded torque and updated log
</commit_message>
<xml_diff>
--- a/Simulink/logs/DryLUPAlog.xlsx
+++ b/Simulink/logs/DryLUPAlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\LUPA\Simulink\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D56AC41-176E-4D12-85EB-0DF8473FEF63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AFDEB3-B6F3-4051-B9B5-5069E8999E2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28704" yWindow="-96" windowWidth="28992" windowHeight="15792" xr2:uid="{C0973FDA-A24E-4A37-9D57-25AD59878F79}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="60">
   <si>
     <t>DryLUPA log</t>
   </si>
@@ -189,7 +189,22 @@
     <t>Chirp2</t>
   </si>
   <si>
-    <t>Chenged to MATLAB release 2022a</t>
+    <t>Changed to MATLAB release 2022a</t>
+  </si>
+  <si>
+    <t>Removed Torque Transducer and installed motor shaft</t>
+  </si>
+  <si>
+    <t>Ramps3</t>
+  </si>
+  <si>
+    <t>Sine3</t>
+  </si>
+  <si>
+    <t>Swapped top and bottom load cell wiring</t>
+  </si>
+  <si>
+    <t>Rewired load cells (Noise reduced)</t>
   </si>
 </sst>
 </file>
@@ -548,11 +563,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638010B8-B628-420C-8BF7-0EC8B4E437D9}">
-  <dimension ref="A1:H445"/>
+  <dimension ref="A1:H448"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F165" sqref="F165"/>
+      <pane ySplit="2" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A177" sqref="A177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3453,9 +3468,12 @@
         <v>50</v>
       </c>
       <c r="C154">
+        <v>1</v>
+      </c>
+      <c r="D154">
         <v>4</v>
       </c>
-      <c r="D154">
+      <c r="E154">
         <v>4</v>
       </c>
     </row>
@@ -3680,81 +3698,217 @@
       <c r="A166" s="1"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A167" s="1"/>
+      <c r="A167" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A168" s="1"/>
+      <c r="A168" s="1">
+        <v>44650</v>
+      </c>
+      <c r="B168" t="s">
+        <v>56</v>
+      </c>
+      <c r="C168">
+        <v>1</v>
+      </c>
+      <c r="D168">
+        <v>2</v>
+      </c>
+      <c r="E168">
+        <v>2</v>
+      </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A169" s="1"/>
+      <c r="A169" s="1">
+        <v>44650</v>
+      </c>
+      <c r="B169" t="s">
+        <v>56</v>
+      </c>
+      <c r="C169">
+        <v>2</v>
+      </c>
+      <c r="D169">
+        <v>4</v>
+      </c>
+      <c r="E169">
+        <v>4</v>
+      </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A170" s="1"/>
+      <c r="A170" s="1">
+        <v>44650</v>
+      </c>
+      <c r="B170" t="s">
+        <v>57</v>
+      </c>
+      <c r="C170">
+        <v>1</v>
+      </c>
+      <c r="D170">
+        <v>0.5</v>
+      </c>
+      <c r="E170">
+        <v>1</v>
+      </c>
+      <c r="F170">
+        <v>2</v>
+      </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A171" s="1"/>
+      <c r="A171" s="1">
+        <v>44650</v>
+      </c>
+      <c r="B171" t="s">
+        <v>57</v>
+      </c>
+      <c r="C171">
+        <v>2</v>
+      </c>
+      <c r="D171">
+        <v>1</v>
+      </c>
+      <c r="E171">
+        <v>2</v>
+      </c>
+      <c r="F171">
+        <v>2</v>
+      </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A172" s="1"/>
+      <c r="A172" s="1">
+        <v>44650</v>
+      </c>
+      <c r="B172" t="s">
+        <v>57</v>
+      </c>
+      <c r="C172">
+        <v>3</v>
+      </c>
+      <c r="D172">
+        <v>1.5</v>
+      </c>
+      <c r="E172">
+        <v>3</v>
+      </c>
+      <c r="F172">
+        <v>2</v>
+      </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A173" s="1"/>
+      <c r="A173" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A174" s="1"/>
+      <c r="A174" s="1">
+        <v>44650</v>
+      </c>
+      <c r="B174" t="s">
+        <v>57</v>
+      </c>
+      <c r="C174">
+        <v>4</v>
+      </c>
+      <c r="D174">
+        <v>2</v>
+      </c>
+      <c r="E174">
+        <v>4</v>
+      </c>
+      <c r="F174">
+        <v>2</v>
+      </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A175" s="1"/>
+      <c r="A175" s="1">
+        <v>44650</v>
+      </c>
+      <c r="B175" t="s">
+        <v>57</v>
+      </c>
+      <c r="C175">
+        <v>5</v>
+      </c>
+      <c r="D175">
+        <v>2.5</v>
+      </c>
+      <c r="E175">
+        <v>5</v>
+      </c>
+      <c r="F175">
+        <v>2</v>
+      </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A176" s="1"/>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A177" s="1"/>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A176" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A177" s="1">
+        <v>44650</v>
+      </c>
+      <c r="B177" t="s">
+        <v>57</v>
+      </c>
+      <c r="C177">
+        <v>6</v>
+      </c>
+      <c r="D177">
+        <v>3</v>
+      </c>
+      <c r="E177">
+        <v>6</v>
+      </c>
+      <c r="F177">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178" s="1"/>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179" s="1"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180" s="1"/>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181" s="1"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182" s="1"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183" s="1"/>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184" s="1"/>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185" s="1"/>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186" s="1"/>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" s="1"/>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188" s="1"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189" s="1"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190" s="1"/>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191" s="1"/>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192" s="1"/>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
@@ -4515,6 +4669,15 @@
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A445" s="1"/>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A446" s="1"/>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A447" s="1"/>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A448" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
added app field data and workspace values to dataset
</commit_message>
<xml_diff>
--- a/Simulink/logs/DryLUPAlog.xlsx
+++ b/Simulink/logs/DryLUPAlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\LUPA\Simulink\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AFDEB3-B6F3-4051-B9B5-5069E8999E2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86696D3-05EA-40B1-B1D9-5F5E959018F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28704" yWindow="-96" windowWidth="28992" windowHeight="15792" xr2:uid="{C0973FDA-A24E-4A37-9D57-25AD59878F79}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="61">
   <si>
     <t>DryLUPA log</t>
   </si>
@@ -204,7 +204,10 @@
     <t>Swapped top and bottom load cell wiring</t>
   </si>
   <si>
-    <t>Rewired load cells (Noise reduced)</t>
+    <t>Changed sign on drawWire</t>
+  </si>
+  <si>
+    <t>Added offset to drawWire</t>
   </si>
 </sst>
 </file>
@@ -563,11 +566,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638010B8-B628-420C-8BF7-0EC8B4E437D9}">
-  <dimension ref="A1:H448"/>
+  <dimension ref="A1:H447"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A177" sqref="A177"/>
+      <pane ySplit="2" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G188" sqref="G188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3842,73 +3845,215 @@
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A176" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A176" s="1">
+        <v>44650</v>
+      </c>
+      <c r="B176" t="s">
+        <v>57</v>
+      </c>
+      <c r="C176">
+        <v>6</v>
+      </c>
+      <c r="D176">
+        <v>3</v>
+      </c>
+      <c r="E176">
+        <v>6</v>
+      </c>
+      <c r="F176">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>44650</v>
       </c>
       <c r="B177" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C177">
+        <v>3</v>
+      </c>
+      <c r="D177">
+        <v>4</v>
+      </c>
+      <c r="E177">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A178" s="1">
+        <v>44650</v>
+      </c>
+      <c r="B178" t="s">
+        <v>56</v>
+      </c>
+      <c r="C178">
+        <v>4</v>
+      </c>
+      <c r="D178">
+        <v>4</v>
+      </c>
+      <c r="E178">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A179" s="1">
+        <v>44650</v>
+      </c>
+      <c r="B179" t="s">
+        <v>56</v>
+      </c>
+      <c r="C179">
+        <v>5</v>
+      </c>
+      <c r="D179">
+        <v>4</v>
+      </c>
+      <c r="E179">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A180" s="1">
+        <v>44650</v>
+      </c>
+      <c r="B180" t="s">
+        <v>56</v>
+      </c>
+      <c r="C180">
         <v>6</v>
       </c>
-      <c r="D177">
-        <v>3</v>
-      </c>
-      <c r="E177">
-        <v>6</v>
-      </c>
-      <c r="F177">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A178" s="1"/>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A179" s="1"/>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A180" s="1"/>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A181" s="1"/>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A182" s="1"/>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A183" s="1"/>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A184" s="1"/>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A185" s="1"/>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A186" s="1"/>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A187" s="1"/>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A188" s="1"/>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D180">
+        <v>4</v>
+      </c>
+      <c r="E180">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A181" s="1">
+        <v>44650</v>
+      </c>
+      <c r="B181" t="s">
+        <v>56</v>
+      </c>
+      <c r="C181">
+        <v>7</v>
+      </c>
+      <c r="D181">
+        <v>4</v>
+      </c>
+      <c r="E181">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A182" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A183" s="1">
+        <v>44650</v>
+      </c>
+      <c r="B183" t="s">
+        <v>56</v>
+      </c>
+      <c r="C183">
+        <v>8</v>
+      </c>
+      <c r="D183">
+        <v>4</v>
+      </c>
+      <c r="E183">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A184" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A185" s="1">
+        <v>44650</v>
+      </c>
+      <c r="B185" t="s">
+        <v>56</v>
+      </c>
+      <c r="C185">
+        <v>9</v>
+      </c>
+      <c r="D185">
+        <v>4</v>
+      </c>
+      <c r="E185">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A186" s="1">
+        <v>44655</v>
+      </c>
+      <c r="B186" t="s">
+        <v>56</v>
+      </c>
+      <c r="C186">
+        <v>10</v>
+      </c>
+      <c r="D186">
+        <v>4</v>
+      </c>
+      <c r="E186">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A187" s="1">
+        <v>44655</v>
+      </c>
+      <c r="B187" t="s">
+        <v>56</v>
+      </c>
+      <c r="C187">
+        <v>11</v>
+      </c>
+      <c r="D187">
+        <v>4</v>
+      </c>
+      <c r="E187">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A188" s="1">
+        <v>44655</v>
+      </c>
+      <c r="B188" t="s">
+        <v>56</v>
+      </c>
+      <c r="C188">
+        <v>12</v>
+      </c>
+      <c r="D188">
+        <v>4</v>
+      </c>
+      <c r="E188">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="1"/>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="1"/>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="1"/>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="1"/>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
@@ -4675,9 +4820,6 @@
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A447" s="1"/>
-    </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A448" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
fixed divide by zero warning with load cells
</commit_message>
<xml_diff>
--- a/Simulink/logs/DryLUPAlog.xlsx
+++ b/Simulink/logs/DryLUPAlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\LUPA\Simulink\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3664F45D-361A-4B16-8B9F-4BDAE1F02678}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5D6622-648D-4905-B6BD-DC189DD9F53F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28704" yWindow="-96" windowWidth="28992" windowHeight="15792" xr2:uid="{C0973FDA-A24E-4A37-9D57-25AD59878F79}"/>
   </bookViews>
@@ -576,7 +576,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G166" sqref="G166"/>
+      <selection pane="bottomLeft" activeCell="G198" sqref="G198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4123,6 +4123,9 @@
       <c r="E192">
         <v>6</v>
       </c>
+      <c r="F192">
+        <v>2</v>
+      </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" s="1"/>

</xml_diff>

<commit_message>
changed filter on EL3351 to 50Hz for both load cells
</commit_message>
<xml_diff>
--- a/Simulink/logs/DryLUPAlog.xlsx
+++ b/Simulink/logs/DryLUPAlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\LUPA\Simulink\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5D6622-648D-4905-B6BD-DC189DD9F53F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3975CA-A0EF-4FC7-B34E-E51EED26A560}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28704" yWindow="-96" windowWidth="28992" windowHeight="15792" xr2:uid="{C0973FDA-A24E-4A37-9D57-25AD59878F79}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="64">
   <si>
     <t>DryLUPA log</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Chirp3</t>
+  </si>
+  <si>
+    <t>Changed bottom load cell to LCM300</t>
   </si>
 </sst>
 </file>
@@ -576,7 +579,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G198" sqref="G198"/>
+      <selection pane="bottomLeft" activeCell="A198" sqref="A198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4127,52 +4130,82 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="1"/>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="1"/>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A195" s="1"/>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A196" s="1"/>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A197" s="1"/>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A195" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A196" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B196" t="s">
+        <v>56</v>
+      </c>
+      <c r="C196">
+        <v>19</v>
+      </c>
+      <c r="D196">
+        <v>2</v>
+      </c>
+      <c r="E196">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A197" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B197" t="s">
+        <v>56</v>
+      </c>
+      <c r="C197">
+        <v>20</v>
+      </c>
+      <c r="D197">
+        <v>3</v>
+      </c>
+      <c r="E197">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="1"/>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="1"/>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="1"/>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="1"/>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="1"/>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="1"/>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="1"/>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" s="1"/>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" s="1"/>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="1"/>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="1"/>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
changed filter on EL3351 to 60Hz for both
</commit_message>
<xml_diff>
--- a/Simulink/logs/DryLUPAlog.xlsx
+++ b/Simulink/logs/DryLUPAlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\LUPA\Simulink\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3975CA-A0EF-4FC7-B34E-E51EED26A560}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B0F461-7100-4F76-87BE-D5F8490B0E67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28704" yWindow="-96" windowWidth="28992" windowHeight="15792" xr2:uid="{C0973FDA-A24E-4A37-9D57-25AD59878F79}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="67">
   <si>
     <t>DryLUPA log</t>
   </si>
@@ -217,6 +217,15 @@
   </si>
   <si>
     <t>Changed bottom load cell to LCM300</t>
+  </si>
+  <si>
+    <t>Changed filters on EL3351 to 60Hz</t>
+  </si>
+  <si>
+    <t>Changed filters on EL3351 to 50Hz</t>
+  </si>
+  <si>
+    <t>Changed filters on EL3351 to 500Hz</t>
   </si>
 </sst>
 </file>
@@ -575,11 +584,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638010B8-B628-420C-8BF7-0EC8B4E437D9}">
-  <dimension ref="A1:H447"/>
+  <dimension ref="A1:H449"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A198" sqref="A198"/>
+      <pane ySplit="2" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A204" sqref="A204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4142,20 +4151,8 @@
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A196" s="1">
-        <v>44706</v>
-      </c>
-      <c r="B196" t="s">
-        <v>56</v>
-      </c>
-      <c r="C196">
-        <v>19</v>
-      </c>
-      <c r="D196">
-        <v>2</v>
-      </c>
-      <c r="E196">
-        <v>2</v>
+      <c r="A196" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
@@ -4166,35 +4163,109 @@
         <v>56</v>
       </c>
       <c r="C197">
+        <v>19</v>
+      </c>
+      <c r="D197">
+        <v>2</v>
+      </c>
+      <c r="E197">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A198" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B198" t="s">
+        <v>56</v>
+      </c>
+      <c r="C198">
         <v>20</v>
       </c>
-      <c r="D197">
-        <v>3</v>
-      </c>
-      <c r="E197">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A198" s="1"/>
+      <c r="D198">
+        <v>3</v>
+      </c>
+      <c r="E198">
+        <v>3</v>
+      </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A199" s="1"/>
+      <c r="A199" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A200" s="1"/>
+      <c r="A200" s="1">
+        <v>44708</v>
+      </c>
+      <c r="B200" t="s">
+        <v>56</v>
+      </c>
+      <c r="C200">
+        <v>21</v>
+      </c>
+      <c r="D200">
+        <v>2</v>
+      </c>
+      <c r="E200">
+        <v>2</v>
+      </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A201" s="1"/>
+      <c r="A201" s="1">
+        <v>44708</v>
+      </c>
+      <c r="B201" t="s">
+        <v>56</v>
+      </c>
+      <c r="C201">
+        <v>22</v>
+      </c>
+      <c r="D201">
+        <v>4</v>
+      </c>
+      <c r="E201">
+        <v>4</v>
+      </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A202" s="1"/>
+      <c r="A202" s="1">
+        <v>44708</v>
+      </c>
+      <c r="B202" t="s">
+        <v>56</v>
+      </c>
+      <c r="C202">
+        <v>23</v>
+      </c>
+      <c r="D202">
+        <v>2</v>
+      </c>
+      <c r="E202">
+        <v>2</v>
+      </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A203" s="1"/>
+      <c r="A203" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A204" s="1"/>
+      <c r="A204" s="1">
+        <v>44708</v>
+      </c>
+      <c r="B204" t="s">
+        <v>56</v>
+      </c>
+      <c r="C204">
+        <v>24</v>
+      </c>
+      <c r="D204">
+        <v>2</v>
+      </c>
+      <c r="E204">
+        <v>2</v>
+      </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" s="1"/>
@@ -4924,6 +4995,12 @@
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A447" s="1"/>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A448" s="1"/>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A449" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>